<commit_message>
feat(CMPF-1037) 매뉴얼 작성 중
</commit_message>
<xml_diff>
--- a/modules/core/template-based-excel-generator/src/test/resources/templates/template.xlsx
+++ b/modules/core/template-based-excel-generator/src/test/resources/templates/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyh/dev/mylib/kotlin/kotlin-common-library/modules/core/template-based-excel-generator/src/test/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC8F9E3-2D00-2A43-8DA6-447221CE9309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E363118-3845-8448-825D-31278CF99A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="600" windowWidth="35440" windowHeight="27520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="600" windowWidth="35440" windowHeight="27520" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="세로 확장(기본형)" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="셀병합" sheetId="3" r:id="rId3"/>
     <sheet name="Named Range" sheetId="4" r:id="rId4"/>
     <sheet name="확장 함수" sheetId="5" r:id="rId5"/>
+    <sheet name="멀티 반복" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="employeeList">'Named Range'!$A$6:$C$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="305" r:id="rId6"/>
+    <pivotCache cacheId="33" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="42">
   <si>
     <t>${title}</t>
   </si>
@@ -192,6 +193,30 @@
   </si>
   <si>
     <t>${repeat(collection=employees, range=employeeList, var=emp)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>부서명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인원</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사무실</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${dep.name}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${dep.members}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${dep.office}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -393,7 +418,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -474,13 +499,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="좋음" xfId="1" builtinId="26"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="하이퍼링크" xfId="2" builtinId="8"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2173,7 +2219,49 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B913C3A8-83B3-D24B-8F4B-0985F48AA6EC}" name="피벗 테이블3" cacheId="305" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" grandTotalCaption="총" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="직급">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D345E0-1F9E-3542-9E98-DBF333DED568}" name="피벗 테이블2" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="M6:N8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="개수 : 이름" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B913C3A8-83B3-D24B-8F4B-0985F48AA6EC}" name="피벗 테이블3" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" grandTotalCaption="총" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="직급">
   <location ref="I6:K8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -2217,17 +2305,17 @@
     <dataField name="평균 급여" fld="2" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="15">
-    <format dxfId="18">
+    <format dxfId="20">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="18">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2237,7 +2325,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="17">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2247,7 +2335,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="16">
       <pivotArea field="1" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2256,7 +2344,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="15">
       <pivotArea field="1" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2265,29 +2353,43 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="14">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
             <x v="0"/>
             <x v="1"/>
           </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
@@ -2299,20 +2401,6 @@
       </pivotArea>
     </format>
     <format dxfId="6">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="5">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -2376,48 +2464,6 @@
       </pivotArea>
     </chartFormat>
   </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D345E0-1F9E-3542-9E98-DBF333DED568}" name="피벗 테이블2" cacheId="305" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="M6:N8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="개수 : 이름" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -2772,7 +2818,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -2927,7 +2973,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2946,7 +2992,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -3190,7 +3236,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3316,7 +3362,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3333,8 +3379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08831A7-1533-E146-BAEE-6768589D142B}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -3445,7 +3491,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3456,4 +3502,173 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F638820-2251-9142-BA78-FEA771EC85A4}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" customWidth="1"/>
+    <col min="5" max="6" width="20" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="50" customHeight="1">
+      <c r="A1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="C1" ca="1">TBEG_IMAGE(ci)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" t="e" cm="1">
+        <f t="array" aca="1" ref="E1" ca="1">TBEG_IMAGE(logo)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F1" s="24" t="str">
+        <f>HYPERLINK("${url}", "${linkText}")</f>
+        <v>${linkText}</v>
+      </c>
+      <c r="G1" s="24"/>
+    </row>
+    <row r="2" spans="1:8" ht="32" customHeight="1">
+      <c r="A2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="e" cm="1">
+        <f t="array" aca="1" ref="A4" ca="1">TBEG_REPEAT(employees, A6:C6, emp)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <f>SUM(C6)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="e" cm="1">
+        <f t="array" aca="1" ref="F10" ca="1">TBEG_REPEAT(departure, F12:H12, dep)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="F11" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="F12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="F8:H8"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThanOrEqual">
+      <formula>6000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+      <formula>6000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{502598B2-4BD2-DC4E-BC82-1B54723E7A58}">
+      <formula1>"사원, 대리, 과장, 차장, 부장"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(CMPF-1037) 멀티 repeat 처리
</commit_message>
<xml_diff>
--- a/modules/core/template-based-excel-generator/src/test/resources/templates/template.xlsx
+++ b/modules/core/template-based-excel-generator/src/test/resources/templates/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyh/dev/mylib/kotlin/kotlin-common-library/modules/core/template-based-excel-generator/src/test/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E363118-3845-8448-825D-31278CF99A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F52980D-A818-7544-879B-0F59D5594B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="600" windowWidth="35440" windowHeight="27520" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="10140" windowWidth="35440" windowHeight="27520" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="세로 확장(기본형)" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="셀병합" sheetId="3" r:id="rId3"/>
     <sheet name="Named Range" sheetId="4" r:id="rId4"/>
     <sheet name="확장 함수" sheetId="5" r:id="rId5"/>
-    <sheet name="멀티 반복" sheetId="6" r:id="rId6"/>
+    <sheet name="멀티 반복" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="employeeList">'Named Range'!$A$6:$C$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="33" r:id="rId7"/>
+    <pivotCache cacheId="116" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
   <si>
     <t>${title}</t>
   </si>
@@ -217,6 +217,22 @@
   </si>
   <si>
     <t>${dep.office}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${secondTitle}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>안녕하세요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${image(ci, C11, 0:-1)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${image(ci, B12, 0:-1)}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -478,6 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -499,14 +516,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="좋음" xfId="1" builtinId="26"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="하이퍼링크" xfId="2" builtinId="8"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2219,7 +2245,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D345E0-1F9E-3542-9E98-DBF333DED568}" name="피벗 테이블2" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D345E0-1F9E-3542-9E98-DBF333DED568}" name="피벗 테이블2" cacheId="116" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M6:N8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -2261,7 +2287,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B913C3A8-83B3-D24B-8F4B-0985F48AA6EC}" name="피벗 테이블3" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" grandTotalCaption="총" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="직급">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B913C3A8-83B3-D24B-8F4B-0985F48AA6EC}" name="피벗 테이블3" cacheId="116" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" grandTotalCaption="총" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="직급">
   <location ref="I6:K8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -2305,17 +2331,17 @@
     <dataField name="평균 급여" fld="2" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="15">
-    <format dxfId="20">
+    <format dxfId="21">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="20">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2325,7 +2351,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="18">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2335,7 +2361,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="17">
       <pivotArea field="1" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2344,7 +2370,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="16">
       <pivotArea field="1" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2353,29 +2379,36 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="15">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="13">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="12">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
             <x v="0"/>
             <x v="1"/>
           </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
@@ -2394,13 +2427,6 @@
       </pivotArea>
     </format>
     <format dxfId="7">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -2834,29 +2860,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="50" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="24" t="str">
+      <c r="F1" s="25" t="str">
         <f>HYPERLINK("${url}", "${linkText}")</f>
         <v>${linkText}</v>
       </c>
-      <c r="G1" s="24"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:14" ht="32" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
@@ -2973,7 +2999,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3003,26 +3029,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="21" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="22"/>
       <c r="F1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="32" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
@@ -3089,26 +3115,26 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="21"/>
+      <c r="C23" s="22"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" t="s">
@@ -3149,24 +3175,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="50" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="32" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -3179,7 +3205,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -3188,14 +3214,14 @@
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="26"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -3204,7 +3230,7 @@
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="21"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="12" t="s">
         <v>7</v>
       </c>
@@ -3236,7 +3262,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3254,7 +3280,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -3270,29 +3296,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="50" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="24" t="str">
+      <c r="F1" s="25" t="str">
         <f>HYPERLINK("${url}", "${linkText}")</f>
         <v>${linkText}</v>
       </c>
-      <c r="G1" s="24"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="32" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
@@ -3362,11 +3388,11 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{235B57F8-47F7-C648-87B5-9EAD463C6935}">
       <formula1>"사원, 대리, 과장, 차장, 부장"</formula1>
     </dataValidation>
@@ -3396,31 +3422,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="50" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="21" t="e" cm="1">
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="C1" ca="1">TBEG_IMAGE(ci)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" t="e" cm="1">
         <f t="array" aca="1" ref="E1" ca="1">TBEG_IMAGE(logo)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F1" s="24" t="str">
+      <c r="F1" s="25" t="str">
         <f>HYPERLINK("${url}", "${linkText}")</f>
         <v>${linkText}</v>
       </c>
-      <c r="G1" s="24"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="32" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
@@ -3491,7 +3517,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3505,11 +3531,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F638820-2251-9142-BA78-FEA771EC85A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A43BECD-0507-2C4A-8414-95386B902C9F}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -3525,31 +3551,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="50" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="21" t="e" cm="1">
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="e" cm="1">
         <f t="array" aca="1" ref="C1" ca="1">TBEG_IMAGE(ci)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" t="e" cm="1">
         <f t="array" aca="1" ref="E1" ca="1">TBEG_IMAGE(logo)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F1" s="24" t="str">
+      <c r="F1" s="25" t="str">
         <f>HYPERLINK("${url}", "${linkText}")</f>
         <v>${linkText}</v>
       </c>
-      <c r="G1" s="24"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="32" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -3561,6 +3587,10 @@
         <f t="array" aca="1" ref="A4" ca="1">TBEG_REPEAT(employees, A6:C6, emp)</f>
         <v>#NAME?</v>
       </c>
+      <c r="E4" t="e" cm="1">
+        <f t="array" aca="1" ref="E4" ca="1">TBEG_REPEAT(department, B10:D10, dep)</f>
+        <v>#NAME?</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
@@ -3573,6 +3603,9 @@
         <v>5</v>
       </c>
       <c r="D5" s="2"/>
+      <c r="E5" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
@@ -3586,7 +3619,12 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="F7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
@@ -3596,11 +3634,11 @@
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="F8" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -3615,22 +3653,28 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="B10" t="s">
-        <v>28</v>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="F10" t="e" cm="1">
-        <f t="array" aca="1" ref="F10" ca="1">TBEG_REPEAT(departure, F12:H12, dep)</f>
+        <f t="array" aca="1" ref="F10" ca="1">TBEG_REPEAT(department, F12:H12, dep)</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3655,20 +3699,26 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="greaterThanOrEqual">
+      <formula>6000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{502598B2-4BD2-DC4E-BC82-1B54723E7A58}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{8A349DEA-6EF6-A946-B7AB-4BE030A7F82F}">
       <formula1>"사원, 대리, 과장, 차장, 부장"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(CMPF-1037) 추가 버그 처리
</commit_message>
<xml_diff>
--- a/modules/core/template-based-excel-generator/src/test/resources/templates/template.xlsx
+++ b/modules/core/template-based-excel-generator/src/test/resources/templates/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyh/dev/mylib/kotlin/kotlin-common-library/modules/core/template-based-excel-generator/src/test/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F52980D-A818-7544-879B-0F59D5594B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3137AC7-0E48-B844-AE51-67DB68FEB4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="10140" windowWidth="35440" windowHeight="27520" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="70260" yWindow="-3400" windowWidth="20980" windowHeight="17020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="세로 확장(기본형)" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="116" r:id="rId7"/>
+    <pivotCache cacheId="118" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="46">
   <si>
     <t>${title}</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>총원:</t>
-  </si>
-  <si>
-    <t>${employees.size()}명</t>
   </si>
   <si>
     <t>(주)휴넷 보고서</t>
@@ -134,10 +131,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${repeat(collection=employees, range=A7:b8, var=emp)}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>총합계</t>
   </si>
   <si>
@@ -148,10 +141,6 @@
   </si>
   <si>
     <t>합계 급여</t>
-  </si>
-  <si>
-    <t>${employees.size()}명</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>행 레이블</t>
@@ -233,6 +222,18 @@
   </si>
   <si>
     <t>${image(ci, B12, 0:-1)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${size(employees)}명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${repeat(collection=mergedEmployees, range=A7:b8, var=emp)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${size(mergedEmployees)}명</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2245,7 +2246,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D345E0-1F9E-3542-9E98-DBF333DED568}" name="피벗 테이블2" cacheId="116" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D345E0-1F9E-3542-9E98-DBF333DED568}" name="피벗 테이블2" cacheId="118" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M6:N8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -2287,7 +2288,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B913C3A8-83B3-D24B-8F4B-0985F48AA6EC}" name="피벗 테이블3" cacheId="116" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" grandTotalCaption="총" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="직급">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B913C3A8-83B3-D24B-8F4B-0985F48AA6EC}" name="피벗 테이블3" cacheId="118" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" grandTotalCaption="총" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="직급">
   <location ref="I6:K8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -2861,11 +2862,11 @@
   <sheetData>
     <row r="1" spans="1:14" ht="50" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" t="s">
@@ -2886,12 +2887,12 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2908,7 +2909,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>6</v>
@@ -2918,22 +2919,22 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" t="s">
         <v>23</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -2958,10 +2959,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J8" s="16">
         <v>0</v>
@@ -2970,7 +2971,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -2978,7 +2979,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>SUM(C6)</f>
@@ -2987,7 +2988,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="B10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3018,7 +3019,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -3030,7 +3031,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="50" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -3039,7 +3040,7 @@
       </c>
       <c r="E1" s="22"/>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="32" customHeight="1">
@@ -3052,12 +3053,12 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1">
@@ -3065,7 +3066,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="11"/>
     </row>
@@ -3078,7 +3079,7 @@
       </c>
       <c r="E6" s="5"/>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3089,7 +3090,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F7">
         <f>SUM(B7)</f>
@@ -3101,22 +3102,22 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="B23" s="22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C23" s="22"/>
     </row>
@@ -3138,7 +3139,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="B30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3163,8 +3164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA2B50C-AA25-8B49-B0CA-84B6326704E6}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -3176,7 +3177,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="50" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="22" t="s">
@@ -3196,17 +3197,17 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="9" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>4</v>
@@ -3216,13 +3217,13 @@
     <row r="6" spans="1:5">
       <c r="A6" s="27"/>
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
@@ -3240,12 +3241,12 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <f>SUM(B8)</f>
@@ -3280,7 +3281,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -3297,11 +3298,11 @@
   <sheetData>
     <row r="1" spans="1:7" ht="50" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" t="s">
@@ -3322,12 +3323,12 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3344,7 +3345,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>6</v>
@@ -3354,7 +3355,7 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3362,12 +3363,12 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>SUM(C6)</f>
@@ -3376,7 +3377,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3406,7 +3407,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -3423,7 +3424,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="50" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="22" t="e" cm="1">
@@ -3450,7 +3451,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3473,7 +3474,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>6</v>
@@ -3483,20 +3484,21 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
+      <c r="B8" t="e" cm="1">
+        <f t="array" aca="1" ref="B8" ca="1">TBEG_SIZE(employees)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>SUM(C6)</f>
@@ -3505,7 +3507,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3521,7 +3523,7 @@
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{97721A6B-7218-C449-B371-110B1AD21D18}">
       <formula1>"사원, 대리, 과장, 차장, 부장"</formula1>
     </dataValidation>
@@ -3534,8 +3536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A43BECD-0507-2C4A-8414-95386B902C9F}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -3552,7 +3554,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="50" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="22" t="e" cm="1">
@@ -3579,7 +3581,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3588,7 +3590,7 @@
         <v>#NAME?</v>
       </c>
       <c r="E4" t="e" cm="1">
-        <f t="array" aca="1" ref="E4" ca="1">TBEG_REPEAT(department, B10:D10, dep)</f>
+        <f t="array" aca="1" ref="E4" ca="1">TBEG_REPEAT(departments, B10:D10, dep)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -3604,12 +3606,12 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>6</v>
@@ -3619,12 +3621,12 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="F7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
@@ -3632,61 +3634,61 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>SUM(C6)</f>
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="B10" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F10" t="e" cm="1">
-        <f t="array" aca="1" ref="F10" ca="1">TBEG_REPEAT(department, F12:H12, dep)</f>
+        <f t="array" aca="1" ref="F10" ca="1">TBEG_REPEAT(departments, F12:H12, dep)</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="F11" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="F12" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3713,7 +3715,7 @@
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{8A349DEA-6EF6-A946-B7AB-4BE030A7F82F}">
       <formula1>"사원, 대리, 과장, 차장, 부장"</formula1>
     </dataValidation>

</xml_diff>